<commit_message>
reorganized for netlify deployment
</commit_message>
<xml_diff>
--- a/Small_Fry_Test_Cases .xlsx
+++ b/Small_Fry_Test_Cases .xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andymckerrow/Helio/sandbox/Test_Plan_SmallFry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andymckerrow/Helio/sandbox/Test_Plan_SmallFry/test_plan_smallfry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D15C8223-53C2-3349-B6CA-96A92C063C11}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BD94DF-A77C-934A-86C9-68080C24F175}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="39" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1360" windowWidth="27360" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="27360" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>